<commit_message>
pre machine learning, adding more data
</commit_message>
<xml_diff>
--- a/US Core Inflation Forecast.xlsx
+++ b/US Core Inflation Forecast.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Science Project\US Core Inflation Forecast\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Science Projects\US_Core_Inflation_Forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52776673-B68E-4AD4-AACC-6CFE59AAF121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86DFEFB-5549-4618-8F66-FC1E4E4771A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Links" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>CPI Core SA (CPILFESL)</t>
   </si>
@@ -42,12 +42,6 @@
   </si>
   <si>
     <t>Released Date</t>
-  </si>
-  <si>
-    <t>https://fred.stlouisfed.org/series/CPILFESL</t>
-  </si>
-  <si>
-    <t>CPI Core SA</t>
   </si>
   <si>
     <t>CPI Core NSA</t>
@@ -109,15 +103,45 @@
   <si>
     <t>https://fred.stlouisfed.org/series/M2NS</t>
   </si>
+  <si>
+    <t>Capacity Utilization</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/series/TCU</t>
+  </si>
+  <si>
+    <t>Manufacturing New Orders</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/series/UMTMNO</t>
+  </si>
+  <si>
+    <t>Nonfarm Employment</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/series/PAYNSA</t>
+  </si>
+  <si>
+    <t>Unemployment Rate SA</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/series/UNRATE</t>
+  </si>
+  <si>
+    <t>Retail Trade</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/series/RSXFSN</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="mm/yyyy"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="mm/yyyy"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -169,13 +193,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
@@ -463,92 +487,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F10B23D-8518-4D05-A1FF-DF7DE7CA0421}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{19966D2C-9EE4-4232-9337-A0A5BBB544BA}"/>
-    <hyperlink ref="B8" r:id="rId2" xr:uid="{2E8479FB-6BE6-4942-AA23-FE06879B08E8}"/>
-    <hyperlink ref="B2" r:id="rId3" xr:uid="{197A49DE-FFA7-4505-A59D-2F88F74BC9C2}"/>
-    <hyperlink ref="B1" r:id="rId4" xr:uid="{4EC4A8D4-3388-4899-9C63-9E39C81ADB0C}"/>
-    <hyperlink ref="B3" r:id="rId5" xr:uid="{A6FAD13D-5675-46DA-915A-607272F85BF4}"/>
-    <hyperlink ref="B4" r:id="rId6" xr:uid="{C20202CB-034A-4E75-9C36-FCFE0DED9C2D}"/>
-    <hyperlink ref="B5" r:id="rId7" xr:uid="{5B1DF681-C934-48BF-A1B9-87685EED064E}"/>
-    <hyperlink ref="B6" r:id="rId8" xr:uid="{72EAA3C5-6E05-4CC9-B52A-BDD891A16DB0}"/>
+    <hyperlink ref="B12" r:id="rId1" xr:uid="{2E8479FB-6BE6-4942-AA23-FE06879B08E8}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{197A49DE-FFA7-4505-A59D-2F88F74BC9C2}"/>
+    <hyperlink ref="B1" r:id="rId3" xr:uid="{4EC4A8D4-3388-4899-9C63-9E39C81ADB0C}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{A6FAD13D-5675-46DA-915A-607272F85BF4}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{C20202CB-034A-4E75-9C36-FCFE0DED9C2D}"/>
+    <hyperlink ref="B5" r:id="rId6" xr:uid="{5B1DF681-C934-48BF-A1B9-87685EED064E}"/>
+    <hyperlink ref="B6" r:id="rId7" xr:uid="{72EAA3C5-6E05-4CC9-B52A-BDD891A16DB0}"/>
+    <hyperlink ref="B7" r:id="rId8" xr:uid="{1DC1F6F0-5712-4BE3-A378-3828909F1F92}"/>
+    <hyperlink ref="B8" r:id="rId9" xr:uid="{CD4097DB-914B-408B-BB12-5F6C91AC3E10}"/>
+    <hyperlink ref="B9" r:id="rId10" xr:uid="{42D2F30F-2365-4C88-9C11-A311018E9004}"/>
+    <hyperlink ref="B10" r:id="rId11" xr:uid="{03A04289-86CB-40C2-806C-3C5632BFDB6E}"/>
+    <hyperlink ref="B11" r:id="rId12" xr:uid="{B1C7B9A6-ED87-4106-A9FC-68C05D1738A2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -558,7 +618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K781"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A762" workbookViewId="0">
+    <sheetView topLeftCell="A762" workbookViewId="0">
       <selection activeCell="F784" sqref="F784"/>
     </sheetView>
   </sheetViews>
@@ -586,31 +646,31 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>